<commit_message>
update xlsx download front pages and re-run/deploy pipeline/app
</commit_message>
<xml_diff>
--- a/data/downloadable_data_templates/iTRAQI front page - ASGS 2011 SA1.xlsx
+++ b/data/downloadable_data_templates/iTRAQI front page - ASGS 2011 SA1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Research\Projects\health\jti_research_data\jti_susanna\TRAQI\Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parsonrr\Documents\R_projects\iTRAQI-analyses\data\downloadable_data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D60A13-D6F3-40EA-9B7F-64E45A223B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93207B-1DD0-46EF-97B4-42B462D9DE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="315" windowWidth="28800" windowHeight="15435" xr2:uid="{86182286-1493-44DE-8FB8-1686E910A6F3}"/>
+    <workbookView xWindow="465" yWindow="3060" windowWidth="29925" windowHeight="17790" xr2:uid="{86182286-1493-44DE-8FB8-1686E910A6F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Front page" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Suggested citation</t>
   </si>
@@ -46,9 +46,6 @@
     <t>for moderate to severe traumatic brain injury</t>
   </si>
   <si>
-    <t>Jamieson Trauma Institute, Retrieval Services Queensland and Queensland University of Technology, 2022. iTRAQI: injury Treatment &amp; Rehabilitation Accessibility Queensland Index, version 1.2. Available from: https://access.healthequity.link/ Accessed [date]</t>
-  </si>
-  <si>
     <t>Methods</t>
   </si>
   <si>
@@ -64,33 +61,12 @@
     <t>Transport to rehabilitation</t>
   </si>
   <si>
-    <t xml:space="preserve">Only road transport was considered, since these would be people visiting the patient. Road driving times were calculated using ArcGIS Online assuming off-peak driving conditions. </t>
-  </si>
-  <si>
-    <t>1.     Patient assumed to have met the Queensland Ambulance Service, pre-hospital trauma by-pass guideline. </t>
-  </si>
-  <si>
-    <t>2.     One hour road transport boundaries calculated using off-peak and non-emergency driving conditions through ArcGIS Online.</t>
-  </si>
-  <si>
-    <t>3.     Transport destination assumptions: </t>
-  </si>
-  <si>
     <t>a.     Directly transport to a major trauma service if road transport time is within 60 minutes. </t>
   </si>
   <si>
-    <t>b.     If greater than 60 minutes drive time to a major trauma service, transport to the highest-level regional trauma service if within 60 minutes. </t>
-  </si>
-  <si>
     <t>c.     If greater than 60 minutes road transport from a major or regional trauma service, transport to the closest hospital. In the event this occurs, immediately notify Retrieval Services Queensland. </t>
   </si>
   <si>
-    <t>4.     Limited consideration given to pre-hospital and aeromedical expertise where the incident occurred at the one-hour road drive time boundary of a major or regional trauma service. </t>
-  </si>
-  <si>
-    <t>5.     Road transport time was included only if the initial destination was a regional or major trauma service.  </t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -100,10 +76,97 @@
     <t>by ASGS 2011 Statistical Area level 1 (SA1)</t>
   </si>
   <si>
-    <t>Both air and road retrievals were included, as appropriate.</t>
-  </si>
-  <si>
     <t>For 441 locations, travel time was calculated to acute care, and driving time to rehabilitation centres. These were interpolated using ordinary kriging to cover all of Queensland as a continuous measure. The median travel time across an SA1 was assigned as the estimate, and provided with the range of travel times in this area.</t>
+  </si>
+  <si>
+    <t>Jamieson Trauma Institute, Retrieval Services Queensland and Queensland University of Technology, 2024. iTRAQI: injury Treatment &amp; Rehabilitation Accessibility Queensland Index, version 2.0. Available from: https://access.healthequity.link/ Accessed [date]</t>
+  </si>
+  <si>
+    <t>This was a mix of air and road retrievals, as would be considered in practice.</t>
+  </si>
+  <si>
+    <t>1.     Patient assumed to have met the Queensland Ambulance Service, pre-hospital trauma by-pass guideline.</t>
+  </si>
+  <si>
+    <t>2.     One hour road transport boundaries calculated using off-peak and non-emergency driving conditions.</t>
+  </si>
+  <si>
+    <t>3.     Response to an acute incident location has the following assumptions:</t>
+  </si>
+  <si>
+    <t>b.     Where ArcGIS Pro calculated an ambulance road transport time of greater than 10 minutes, the additional travel (beyond 10 minutes) time was included (i.e. if the total travel time to an incident was 15 minutes, 5 minutes travel time was added to point 3.a).</t>
+  </si>
+  <si>
+    <t>4.     Transport destination assumptions:</t>
+  </si>
+  <si>
+    <t>1.     National Triple Zero (000) call routing to the ambulance service in Queensland;</t>
+  </si>
+  <si>
+    <t>2.     Time for an Emergency Medical Dispatcher to answer the call;</t>
+  </si>
+  <si>
+    <t>3.     Triple Zero (000) call-taking procedure and/or RSQ coordination;</t>
+  </si>
+  <si>
+    <t>4.     Dispatch of primary ambulance or aeromedical platform (i.e. notification of responding platform/service);</t>
+  </si>
+  <si>
+    <t>5.     Time for health professionals to respond (i.e. receive an alert, walk to the ambulance/platform, set up navigation, etc.); and</t>
+  </si>
+  <si>
+    <t>6.     Up to 10 minutes of road travel time.</t>
+  </si>
+  <si>
+    <t>a.     Directly transport to a major trauma service (also referred to as a ‘neurosurgical centre’ in the case of moderate-severe TBI) if road transport time is within 60 minutes.</t>
+  </si>
+  <si>
+    <t>b.     If greater than 60 minutes road transport time to a major trauma service, transport to the highest-level regional trauma service if within 60 minutes.</t>
+  </si>
+  <si>
+    <t>c.     If greater than 60 minutes road transport from a major or regional trauma service, transport to the closest hospital. In the event this occurs, immediately notify Retrieval Services Queensland.</t>
+  </si>
+  <si>
+    <t>5.     Every road ambulance response was assigned 20 minutes of time on-scene for paramedics to assess, manage and extricate the patient.</t>
+  </si>
+  <si>
+    <t>6.     Limited consideration given to pre-hospital and aeromedical expertise where the incident occurred at the one-hour road drive time boundary of a major or regional trauma service.</t>
+  </si>
+  <si>
+    <t>7.     Road transport time was included only if the initial destination was a regional or major trauma service.</t>
+  </si>
+  <si>
+    <t>Aeromedical transport assumptions:</t>
+  </si>
+  <si>
+    <t>1.     An aeromedical response (fixed wing, rotary wing, or a combination) is available at the closest home base, with no duty hours or weather restrictions, based on current aircraft locations and types.</t>
+  </si>
+  <si>
+    <t>2.     Transport as rapidly as possible to either Brisbane, Gold Coast or Townsville airports for fixed wing responses, or PAH, RBWH, GCUH or TUH for rotary wing responses.</t>
+  </si>
+  <si>
+    <t>a.     The in-flight time for each aeromedical leg was provided by RFDS or the RSQ Rotary Advisor, based on aircraft type at each base and calculated times based on direct flight paths</t>
+  </si>
+  <si>
+    <t>3.     Standardised response times were estimated by one of the investigators (CG) and validated by consensus opinion from other senior medical staff at RSQ. These included:</t>
+  </si>
+  <si>
+    <t>a.     Coordination and tasking by RSQ (see 3a above under ’Road transport assumptions)</t>
+  </si>
+  <si>
+    <t>b.     Response times by aeromedical teams [rotary wing (15 minutes) and fixed wing (60 minutes)]</t>
+  </si>
+  <si>
+    <t>c.     Standardised on-scene times [rotary wing (60 minutes) and fixed wing (120 minutes)]</t>
+  </si>
+  <si>
+    <t>d.     Where a patient was initially transported to a regional trauma service, 120 minutes was added to the patient journey. This time allows for initial triage, assessment and management of the patient at the regional trauma service prior to transport to a major trauma service</t>
+  </si>
+  <si>
+    <t>Based on driving times, calculated using ArcGIS Online, using established speed limits and road networks, and using ‘off-peak’ traffic conditions.</t>
+  </si>
+  <si>
+    <t>4.     No restrictions to destination facilities, such as access block.</t>
   </si>
 </sst>
 </file>
@@ -111,7 +174,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -202,10 +265,10 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -217,50 +280,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="13"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="17"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -299,9 +365,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -339,7 +405,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -445,7 +511,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -587,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -595,327 +661,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1B2508-4B4F-4AB7-B781-246B43C03FCE}">
-  <dimension ref="B10:R42"/>
+  <dimension ref="B10:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="12" spans="2:18" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
     </row>
     <row r="13" spans="2:18" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="2:18" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="F14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="17" spans="4:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="4:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="6"/>
+      <c r="D18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="3"/>
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="4:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="3"/>
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="4:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="3"/>
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="4:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="D21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="4:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
+      <c r="D22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
     </row>
     <row r="23" spans="4:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="4:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="4:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="4:16" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-    </row>
-    <row r="26" spans="4:16" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="9" t="s">
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D31" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D32" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D27" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D29" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D30" s="10" t="s">
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D49" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D51" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D52" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D53" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D54" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D56" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D57" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D58" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D59" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D60" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D62" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D31" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D32" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D33" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D34" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D35" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D36" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D37" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D38" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D40" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="4:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-    </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D42" s="15"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+    </row>
+    <row r="63" spans="4:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+    </row>
+    <row r="64" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D64" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="D27:P27"/>
-    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="D62:P62"/>
     <mergeCell ref="D26:N26"/>
-    <mergeCell ref="D41:N41"/>
+    <mergeCell ref="D63:N63"/>
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D10:P10"/>
     <mergeCell ref="D17:P17"/>

</xml_diff>